<commit_message>
well validation between datasets
</commit_message>
<xml_diff>
--- a/raw_data/flow_cytometry/WGS2_ploid_assay.xlsx
+++ b/raw_data/flow_cytometry/WGS2_ploid_assay.xlsx
@@ -16,7 +16,7 @@
     <t>sample name</t>
   </si>
   <si>
-    <t>hap/dip</t>
+    <t>dip_hap_na</t>
   </si>
   <si>
     <t>All Events Count</t>
@@ -268,12 +268,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -537,7 +540,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="41.75"/>
+    <col customWidth="1" min="1" max="1" width="41.75"/>
+    <col customWidth="1" min="2" max="2" width="14.25"/>
     <col customWidth="1" min="4" max="4" width="27.88"/>
   </cols>
   <sheetData>
@@ -545,7 +549,7 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -593,7 +597,7 @@
       <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="3" t="s">
         <v>17</v>
       </c>
       <c r="T1" s="1" t="s">
@@ -608,7 +612,7 @@
       <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="3" t="s">
         <v>22</v>
       </c>
       <c r="Y1" s="1" t="s">
@@ -632,8 +636,8 @@
         <f t="shared" ref="B2:B22" si="1">CONCATENATE(AC2,AD2,AE2)</f>
         <v>WGS2A1</v>
       </c>
-      <c r="C2" s="1" t="str">
-        <f t="shared" ref="C2:C22" si="2">IF(AND(T2&gt;10, Y2&gt;10), "dubious",IF(AND(ISBLANK(T2),ISBLANK(Y2)), "na", IF(T2&gt;Y2, "haploid", IF(Y2&gt;T2, "diploid", "na"))))</f>
+      <c r="C2" s="2" t="str">
+        <f t="shared" ref="C2:C22" si="2">IF(AND(S2&gt;10, X2&gt;10), "dubious",IF(AND(ISBLANK(S2),ISBLANK(X2)), "na", IF(S2&gt;X2, "haploid", IF(X2&gt;S2, "diploid", "na"))))</f>
         <v>diploid</v>
       </c>
       <c r="D2" s="1">
@@ -681,7 +685,7 @@
       <c r="R2" s="1">
         <v>113.76</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="3">
         <v>0.0</v>
       </c>
       <c r="T2" s="1">
@@ -696,7 +700,7 @@
       <c r="W2" s="1">
         <v>0.0</v>
       </c>
-      <c r="X2" s="2">
+      <c r="X2" s="3">
         <v>715.0</v>
       </c>
       <c r="Y2" s="1">
@@ -711,16 +715,16 @@
       <c r="AB2" s="1">
         <v>30.0</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AC2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AD2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AE2" s="5">
+      <c r="AE2" s="6">
         <v>1.0</v>
       </c>
-      <c r="AF2" s="5"/>
+      <c r="AF2" s="6"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
@@ -730,7 +734,7 @@
         <f t="shared" si="1"/>
         <v>WGS2B1</v>
       </c>
-      <c r="C3" s="1" t="str">
+      <c r="C3" s="2" t="str">
         <f t="shared" si="2"/>
         <v>diploid</v>
       </c>
@@ -779,7 +783,7 @@
       <c r="R3" s="1">
         <v>430.62</v>
       </c>
-      <c r="S3" s="2">
+      <c r="S3" s="3">
         <v>0.0</v>
       </c>
       <c r="T3" s="1">
@@ -794,7 +798,7 @@
       <c r="W3" s="1">
         <v>0.0</v>
       </c>
-      <c r="X3" s="2">
+      <c r="X3" s="3">
         <v>538.0</v>
       </c>
       <c r="Y3" s="1">
@@ -809,16 +813,16 @@
       <c r="AB3" s="1">
         <v>66.42</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AC3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AD3" s="4" t="s">
+      <c r="AD3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AE3" s="5">
+      <c r="AE3" s="6">
         <v>1.0</v>
       </c>
-      <c r="AF3" s="5"/>
+      <c r="AF3" s="6"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
@@ -828,7 +832,7 @@
         <f t="shared" si="1"/>
         <v>WGS2C1</v>
       </c>
-      <c r="C4" s="1" t="str">
+      <c r="C4" s="2" t="str">
         <f t="shared" si="2"/>
         <v>diploid</v>
       </c>
@@ -877,7 +881,7 @@
       <c r="R4" s="1">
         <v>30.13</v>
       </c>
-      <c r="S4" s="2">
+      <c r="S4" s="3">
         <v>1.0</v>
       </c>
       <c r="T4" s="1">
@@ -892,7 +896,7 @@
       <c r="W4" s="1">
         <v>0.01</v>
       </c>
-      <c r="X4" s="2">
+      <c r="X4" s="3">
         <v>196.0</v>
       </c>
       <c r="Y4" s="1">
@@ -907,28 +911,28 @@
       <c r="AB4" s="1">
         <v>2.04</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AC4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AD4" s="4" t="s">
+      <c r="AD4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AE4" s="5">
+      <c r="AE4" s="6">
         <v>1.0</v>
       </c>
-      <c r="AF4" s="5"/>
+      <c r="AF4" s="6"/>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="1" t="str">
         <f t="shared" si="1"/>
         <v>WGS2D1</v>
       </c>
-      <c r="C5" s="6" t="str">
+      <c r="C5" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>haploid</v>
+        <v>dubious</v>
       </c>
       <c r="D5" s="1">
         <v>400.0</v>
@@ -975,7 +979,7 @@
       <c r="R5" s="1">
         <v>4.45</v>
       </c>
-      <c r="S5" s="2">
+      <c r="S5" s="3">
         <v>57.0</v>
       </c>
       <c r="T5" s="1">
@@ -990,7 +994,7 @@
       <c r="W5" s="1">
         <v>1.2</v>
       </c>
-      <c r="X5" s="2">
+      <c r="X5" s="3">
         <v>17.0</v>
       </c>
       <c r="Y5" s="1">
@@ -1005,114 +1009,114 @@
       <c r="AB5" s="1">
         <v>0.36</v>
       </c>
-      <c r="AC5" s="3" t="s">
+      <c r="AC5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AD5" s="4" t="s">
+      <c r="AD5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AE5" s="5">
+      <c r="AE5" s="6">
         <v>1.0</v>
       </c>
-      <c r="AF5" s="5"/>
+      <c r="AF5" s="6"/>
     </row>
     <row r="6" ht="17.25" customHeight="1">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="1" t="str">
         <f t="shared" si="1"/>
         <v>WGS2F1</v>
       </c>
-      <c r="C6" s="7" t="str">
+      <c r="C6" s="2" t="str">
         <f t="shared" si="2"/>
         <v>haploid</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="8">
         <v>1288.0</v>
       </c>
-      <c r="E6" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="F6" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="G6" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="H6" s="7">
+      <c r="E6" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="F6" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="G6" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="H6" s="8">
         <v>64.37</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="8">
         <v>159.0</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="8">
         <v>12.34</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="8">
         <v>12.34</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="8">
         <v>12.34</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="8">
         <v>7.95</v>
       </c>
-      <c r="N6" s="7">
+      <c r="N6" s="8">
         <v>140.0</v>
       </c>
-      <c r="O6" s="7">
+      <c r="O6" s="8">
         <v>88.05</v>
       </c>
-      <c r="P6" s="7">
+      <c r="P6" s="8">
         <v>10.87</v>
       </c>
-      <c r="Q6" s="7">
+      <c r="Q6" s="8">
         <v>10.87</v>
       </c>
-      <c r="R6" s="7">
+      <c r="R6" s="8">
         <v>7.0</v>
       </c>
-      <c r="S6" s="8">
+      <c r="S6" s="9">
         <v>19.0</v>
       </c>
-      <c r="T6" s="7">
+      <c r="T6" s="8">
         <v>13.57</v>
       </c>
-      <c r="U6" s="7">
+      <c r="U6" s="8">
         <v>11.95</v>
       </c>
-      <c r="V6" s="7">
+      <c r="V6" s="8">
         <v>1.48</v>
       </c>
-      <c r="W6" s="7">
+      <c r="W6" s="8">
         <v>0.95</v>
       </c>
-      <c r="X6" s="8">
+      <c r="X6" s="9">
         <v>4.0</v>
       </c>
-      <c r="Y6" s="7">
+      <c r="Y6" s="8">
         <v>2.86</v>
       </c>
-      <c r="Z6" s="7">
+      <c r="Z6" s="8">
         <v>2.52</v>
       </c>
-      <c r="AA6" s="7">
+      <c r="AA6" s="8">
         <v>0.31</v>
       </c>
-      <c r="AB6" s="7">
+      <c r="AB6" s="8">
         <v>0.2</v>
       </c>
-      <c r="AC6" s="9" t="s">
+      <c r="AC6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="AD6" s="9" t="s">
+      <c r="AD6" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="AE6" s="10">
+      <c r="AE6" s="11">
         <v>1.0</v>
       </c>
-      <c r="AF6" s="11"/>
+      <c r="AF6" s="12"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
@@ -1122,7 +1126,7 @@
         <f t="shared" si="1"/>
         <v>WGS2F2</v>
       </c>
-      <c r="C7" s="1" t="str">
+      <c r="C7" s="2" t="str">
         <f t="shared" si="2"/>
         <v>haploid</v>
       </c>
@@ -1171,7 +1175,7 @@
       <c r="R7" s="1">
         <v>64.77</v>
       </c>
-      <c r="S7" s="2">
+      <c r="S7" s="3">
         <v>837.0</v>
       </c>
       <c r="T7" s="1">
@@ -1186,7 +1190,7 @@
       <c r="W7" s="1">
         <v>16.58</v>
       </c>
-      <c r="X7" s="2">
+      <c r="X7" s="3">
         <v>9.0</v>
       </c>
       <c r="Y7" s="1">
@@ -1201,114 +1205,114 @@
       <c r="AB7" s="1">
         <v>0.18</v>
       </c>
-      <c r="AC7" s="3" t="s">
+      <c r="AC7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AD7" s="3" t="s">
+      <c r="AD7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AE7" s="12">
+      <c r="AE7" s="13">
         <v>2.0</v>
       </c>
-      <c r="AF7" s="5"/>
+      <c r="AF7" s="6"/>
     </row>
     <row r="8">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B8" s="1" t="str">
         <f t="shared" si="1"/>
         <v>WGS2G2</v>
       </c>
-      <c r="C8" s="7" t="str">
+      <c r="C8" s="2" t="str">
         <f t="shared" si="2"/>
         <v>diploid</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="8">
         <v>1440.0</v>
       </c>
-      <c r="E8" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="F8" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="G8" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="H8" s="7">
+      <c r="E8" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="F8" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="G8" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="H8" s="8">
         <v>14.38</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="8">
         <v>1137.0</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="8">
         <v>78.96</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="8">
         <v>78.96</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8" s="8">
         <v>78.96</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="8">
         <v>11.36</v>
       </c>
-      <c r="N8" s="7">
+      <c r="N8" s="8">
         <v>1005.0</v>
       </c>
-      <c r="O8" s="7">
+      <c r="O8" s="8">
         <v>88.39</v>
       </c>
-      <c r="P8" s="7">
+      <c r="P8" s="8">
         <v>69.79</v>
       </c>
-      <c r="Q8" s="7">
+      <c r="Q8" s="8">
         <v>69.79</v>
       </c>
-      <c r="R8" s="7">
+      <c r="R8" s="8">
         <v>10.04</v>
       </c>
-      <c r="S8" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="T8" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="U8" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="V8" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="W8" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="X8" s="8">
+      <c r="S8" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="T8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="U8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="V8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="W8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="X8" s="9">
         <v>159.0</v>
       </c>
-      <c r="Y8" s="7">
+      <c r="Y8" s="8">
         <v>15.82</v>
       </c>
-      <c r="Z8" s="7">
+      <c r="Z8" s="8">
         <v>13.98</v>
       </c>
-      <c r="AA8" s="7">
+      <c r="AA8" s="8">
         <v>11.04</v>
       </c>
-      <c r="AB8" s="7">
+      <c r="AB8" s="8">
         <v>1.59</v>
       </c>
-      <c r="AC8" s="9" t="s">
+      <c r="AC8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="AD8" s="9" t="s">
+      <c r="AD8" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="AE8" s="13">
+      <c r="AE8" s="14">
         <v>2.0</v>
       </c>
-      <c r="AF8" s="10"/>
+      <c r="AF8" s="11"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
@@ -1318,7 +1322,7 @@
         <f t="shared" si="1"/>
         <v>WGS2A3</v>
       </c>
-      <c r="C9" s="1" t="str">
+      <c r="C9" s="2" t="str">
         <f t="shared" si="2"/>
         <v>diploid</v>
       </c>
@@ -1367,7 +1371,7 @@
       <c r="R9" s="1">
         <v>5.39</v>
       </c>
-      <c r="S9" s="2">
+      <c r="S9" s="3">
         <v>0.0</v>
       </c>
       <c r="T9" s="1">
@@ -1382,7 +1386,7 @@
       <c r="W9" s="1">
         <v>0.0</v>
       </c>
-      <c r="X9" s="2">
+      <c r="X9" s="3">
         <v>34.0</v>
       </c>
       <c r="Y9" s="1">
@@ -1397,114 +1401,114 @@
       <c r="AB9" s="1">
         <v>0.35</v>
       </c>
-      <c r="AC9" s="3" t="s">
+      <c r="AC9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AD9" s="3" t="s">
+      <c r="AD9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AE9" s="12">
+      <c r="AE9" s="13">
         <v>3.0</v>
       </c>
-      <c r="AF9" s="5"/>
+      <c r="AF9" s="6"/>
     </row>
     <row r="10">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="8" t="s">
         <v>42</v>
       </c>
       <c r="B10" s="1" t="str">
         <f t="shared" si="1"/>
         <v>WGS2C3</v>
       </c>
-      <c r="C10" s="7" t="str">
+      <c r="C10" s="2" t="str">
         <f t="shared" si="2"/>
         <v>haploid</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="8">
         <v>304.0</v>
       </c>
-      <c r="E10" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="F10" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="G10" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="H10" s="7">
+      <c r="E10" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="F10" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="G10" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="H10" s="8">
         <v>6.96</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="8">
         <v>187.0</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="8">
         <v>61.51</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="8">
         <v>61.51</v>
       </c>
-      <c r="L10" s="7">
+      <c r="L10" s="8">
         <v>61.51</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="8">
         <v>4.28</v>
       </c>
-      <c r="N10" s="7">
+      <c r="N10" s="8">
         <v>169.0</v>
       </c>
-      <c r="O10" s="7">
+      <c r="O10" s="8">
         <v>90.37</v>
       </c>
-      <c r="P10" s="7">
+      <c r="P10" s="8">
         <v>55.59</v>
       </c>
-      <c r="Q10" s="7">
+      <c r="Q10" s="8">
         <v>55.59</v>
       </c>
-      <c r="R10" s="7">
+      <c r="R10" s="8">
         <v>3.87</v>
       </c>
-      <c r="S10" s="8">
+      <c r="S10" s="9">
         <v>55.0</v>
       </c>
-      <c r="T10" s="7">
+      <c r="T10" s="8">
         <v>32.54</v>
       </c>
-      <c r="U10" s="7">
+      <c r="U10" s="8">
         <v>29.41</v>
       </c>
-      <c r="V10" s="7">
+      <c r="V10" s="8">
         <v>18.09</v>
       </c>
-      <c r="W10" s="7">
+      <c r="W10" s="8">
         <v>1.26</v>
       </c>
-      <c r="X10" s="8">
+      <c r="X10" s="9">
         <v>9.0</v>
       </c>
-      <c r="Y10" s="7">
+      <c r="Y10" s="8">
         <v>5.33</v>
       </c>
-      <c r="Z10" s="7">
+      <c r="Z10" s="8">
         <v>4.81</v>
       </c>
-      <c r="AA10" s="7">
+      <c r="AA10" s="8">
         <v>2.96</v>
       </c>
-      <c r="AB10" s="7">
+      <c r="AB10" s="8">
         <v>0.21</v>
       </c>
-      <c r="AC10" s="9" t="s">
+      <c r="AC10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="AD10" s="9" t="s">
+      <c r="AD10" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="AE10" s="13">
+      <c r="AE10" s="14">
         <v>3.0</v>
       </c>
-      <c r="AF10" s="10"/>
+      <c r="AF10" s="11"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
@@ -1514,7 +1518,7 @@
         <f t="shared" si="1"/>
         <v>WGS2D4</v>
       </c>
-      <c r="C11" s="1" t="str">
+      <c r="C11" s="2" t="str">
         <f t="shared" si="2"/>
         <v>diploid</v>
       </c>
@@ -1563,7 +1567,7 @@
       <c r="R11" s="1">
         <v>561.03</v>
       </c>
-      <c r="S11" s="2">
+      <c r="S11" s="3">
         <v>9.0</v>
       </c>
       <c r="T11" s="1">
@@ -1578,7 +1582,7 @@
       <c r="W11" s="1">
         <v>1.65</v>
       </c>
-      <c r="X11" s="2">
+      <c r="X11" s="3">
         <v>822.0</v>
       </c>
       <c r="Y11" s="1">
@@ -1593,16 +1597,16 @@
       <c r="AB11" s="1">
         <v>151.1</v>
       </c>
-      <c r="AC11" s="3" t="s">
+      <c r="AC11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AD11" s="3" t="s">
+      <c r="AD11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AE11" s="12">
+      <c r="AE11" s="13">
         <v>4.0</v>
       </c>
-      <c r="AF11" s="5"/>
+      <c r="AF11" s="6"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
@@ -1612,7 +1616,7 @@
         <f t="shared" si="1"/>
         <v>WGS2E4</v>
       </c>
-      <c r="C12" s="1" t="str">
+      <c r="C12" s="2" t="str">
         <f t="shared" si="2"/>
         <v>diploid</v>
       </c>
@@ -1661,7 +1665,7 @@
       <c r="R12" s="1">
         <v>112.56</v>
       </c>
-      <c r="S12" s="2">
+      <c r="S12" s="3">
         <v>0.0</v>
       </c>
       <c r="T12" s="1">
@@ -1676,7 +1680,7 @@
       <c r="W12" s="1">
         <v>0.0</v>
       </c>
-      <c r="X12" s="2">
+      <c r="X12" s="3">
         <v>330.0</v>
       </c>
       <c r="Y12" s="1">
@@ -1691,114 +1695,114 @@
       <c r="AB12" s="1">
         <v>10.69</v>
       </c>
-      <c r="AC12" s="3" t="s">
+      <c r="AC12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AD12" s="3" t="s">
+      <c r="AD12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AE12" s="12">
+      <c r="AE12" s="13">
         <v>4.0</v>
       </c>
-      <c r="AF12" s="5"/>
+      <c r="AF12" s="6"/>
     </row>
     <row r="13">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="8" t="s">
         <v>46</v>
       </c>
       <c r="B13" s="1" t="str">
         <f t="shared" si="1"/>
         <v>WGS2F4</v>
       </c>
-      <c r="C13" s="7" t="str">
+      <c r="C13" s="2" t="str">
         <f t="shared" si="2"/>
         <v>haploid</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="8">
         <v>616.0</v>
       </c>
-      <c r="E13" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="F13" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="G13" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="H13" s="7">
+      <c r="E13" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="F13" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="G13" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="H13" s="8">
         <v>22.84</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="8">
         <v>303.0</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="8">
         <v>49.19</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="8">
         <v>49.19</v>
       </c>
-      <c r="L13" s="7">
+      <c r="L13" s="8">
         <v>49.19</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13" s="8">
         <v>11.23</v>
       </c>
-      <c r="N13" s="7">
+      <c r="N13" s="8">
         <v>183.0</v>
       </c>
-      <c r="O13" s="7">
+      <c r="O13" s="8">
         <v>60.4</v>
       </c>
-      <c r="P13" s="7">
+      <c r="P13" s="8">
         <v>29.71</v>
       </c>
-      <c r="Q13" s="7">
+      <c r="Q13" s="8">
         <v>29.71</v>
       </c>
-      <c r="R13" s="7">
+      <c r="R13" s="8">
         <v>6.79</v>
       </c>
-      <c r="S13" s="8">
+      <c r="S13" s="9">
         <v>127.0</v>
       </c>
-      <c r="T13" s="7">
+      <c r="T13" s="8">
         <v>69.4</v>
       </c>
-      <c r="U13" s="7">
+      <c r="U13" s="8">
         <v>41.91</v>
       </c>
-      <c r="V13" s="7">
+      <c r="V13" s="8">
         <v>20.62</v>
       </c>
-      <c r="W13" s="7">
+      <c r="W13" s="8">
         <v>4.71</v>
       </c>
-      <c r="X13" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="Y13" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="Z13" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="AA13" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="AB13" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="AC13" s="9" t="s">
+      <c r="X13" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="Y13" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="Z13" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="AA13" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="AB13" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="AC13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="AD13" s="9" t="s">
+      <c r="AD13" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="AE13" s="13">
+      <c r="AE13" s="14">
         <v>4.0</v>
       </c>
-      <c r="AF13" s="10"/>
+      <c r="AF13" s="11"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
@@ -1808,9 +1812,9 @@
         <f t="shared" si="1"/>
         <v>WGS2B6</v>
       </c>
-      <c r="C14" s="1" t="str">
+      <c r="C14" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>dubious</v>
+        <v>na</v>
       </c>
       <c r="D14" s="1">
         <v>40.0</v>
@@ -1857,7 +1861,7 @@
       <c r="R14" s="1">
         <v>0.0</v>
       </c>
-      <c r="S14" s="2">
+      <c r="S14" s="3">
         <v>0.0</v>
       </c>
       <c r="T14" s="1" t="s">
@@ -1872,7 +1876,7 @@
       <c r="W14" s="1">
         <v>0.0</v>
       </c>
-      <c r="X14" s="2">
+      <c r="X14" s="3">
         <v>0.0</v>
       </c>
       <c r="Y14" s="1" t="s">
@@ -1887,114 +1891,114 @@
       <c r="AB14" s="1">
         <v>0.0</v>
       </c>
-      <c r="AC14" s="3" t="s">
+      <c r="AC14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AD14" s="3" t="s">
+      <c r="AD14" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AE14" s="12">
+      <c r="AE14" s="13">
         <v>6.0</v>
       </c>
-      <c r="AF14" s="5"/>
+      <c r="AF14" s="6"/>
     </row>
     <row r="15">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="8" t="s">
         <v>49</v>
       </c>
       <c r="B15" s="1" t="str">
         <f t="shared" si="1"/>
         <v>WGS2C6</v>
       </c>
-      <c r="C15" s="7" t="str">
+      <c r="C15" s="2" t="str">
         <f t="shared" si="2"/>
         <v>diploid</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="8">
         <v>128.0</v>
       </c>
-      <c r="E15" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="F15" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="G15" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="H15" s="7">
+      <c r="E15" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="F15" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="G15" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="H15" s="8">
         <v>1.28</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="8">
         <v>62.0</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J15" s="8">
         <v>48.44</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K15" s="8">
         <v>48.44</v>
       </c>
-      <c r="L15" s="7">
+      <c r="L15" s="8">
         <v>48.44</v>
       </c>
-      <c r="M15" s="7">
+      <c r="M15" s="8">
         <v>0.62</v>
       </c>
-      <c r="N15" s="7">
+      <c r="N15" s="8">
         <v>56.0</v>
       </c>
-      <c r="O15" s="7">
+      <c r="O15" s="8">
         <v>90.32</v>
       </c>
-      <c r="P15" s="7">
+      <c r="P15" s="8">
         <v>43.75</v>
       </c>
-      <c r="Q15" s="7">
+      <c r="Q15" s="8">
         <v>43.75</v>
       </c>
-      <c r="R15" s="7">
+      <c r="R15" s="8">
         <v>0.56</v>
       </c>
-      <c r="S15" s="8">
+      <c r="S15" s="9">
         <v>1.0</v>
       </c>
-      <c r="T15" s="7">
+      <c r="T15" s="8">
         <v>1.79</v>
       </c>
-      <c r="U15" s="7">
+      <c r="U15" s="8">
         <v>1.61</v>
       </c>
-      <c r="V15" s="7">
+      <c r="V15" s="8">
         <v>0.78</v>
       </c>
-      <c r="W15" s="7">
+      <c r="W15" s="8">
         <v>0.01</v>
       </c>
-      <c r="X15" s="8">
+      <c r="X15" s="9">
         <v>6.0</v>
       </c>
-      <c r="Y15" s="7">
+      <c r="Y15" s="8">
         <v>10.71</v>
       </c>
-      <c r="Z15" s="7">
+      <c r="Z15" s="8">
         <v>9.68</v>
       </c>
-      <c r="AA15" s="7">
+      <c r="AA15" s="8">
         <v>4.69</v>
       </c>
-      <c r="AB15" s="7">
+      <c r="AB15" s="8">
         <v>0.06</v>
       </c>
-      <c r="AC15" s="9" t="s">
+      <c r="AC15" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="AD15" s="9" t="s">
+      <c r="AD15" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="AE15" s="13">
+      <c r="AE15" s="14">
         <v>6.0</v>
       </c>
-      <c r="AF15" s="10"/>
+      <c r="AF15" s="11"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
@@ -2004,7 +2008,7 @@
         <f t="shared" si="1"/>
         <v>WGS2A7</v>
       </c>
-      <c r="C16" s="1" t="str">
+      <c r="C16" s="2" t="str">
         <f t="shared" si="2"/>
         <v>haploid</v>
       </c>
@@ -2053,7 +2057,7 @@
       <c r="R16" s="1">
         <v>1.76</v>
       </c>
-      <c r="S16" s="2">
+      <c r="S16" s="3">
         <v>14.0</v>
       </c>
       <c r="T16" s="1">
@@ -2068,7 +2072,7 @@
       <c r="W16" s="1">
         <v>0.79</v>
       </c>
-      <c r="X16" s="2">
+      <c r="X16" s="3">
         <v>0.0</v>
       </c>
       <c r="Y16" s="1">
@@ -2083,212 +2087,212 @@
       <c r="AB16" s="1">
         <v>0.0</v>
       </c>
-      <c r="AC16" s="3" t="s">
+      <c r="AC16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AD16" s="3" t="s">
+      <c r="AD16" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AE16" s="12">
+      <c r="AE16" s="13">
         <v>7.0</v>
       </c>
-      <c r="AF16" s="5"/>
+      <c r="AF16" s="6"/>
     </row>
     <row r="17">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="8" t="s">
         <v>51</v>
       </c>
       <c r="B17" s="1" t="str">
         <f t="shared" si="1"/>
         <v>WGS2G7</v>
       </c>
-      <c r="C17" s="7" t="str">
+      <c r="C17" s="2" t="str">
         <f t="shared" si="2"/>
         <v>diploid</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="8">
         <v>264.0</v>
       </c>
-      <c r="E17" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="F17" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="G17" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="H17" s="7">
+      <c r="E17" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="F17" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="G17" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="H17" s="8">
         <v>2.64</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="8">
         <v>131.0</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J17" s="8">
         <v>49.62</v>
       </c>
-      <c r="K17" s="7">
+      <c r="K17" s="8">
         <v>49.62</v>
       </c>
-      <c r="L17" s="7">
+      <c r="L17" s="8">
         <v>49.62</v>
       </c>
-      <c r="M17" s="7">
+      <c r="M17" s="8">
         <v>1.31</v>
       </c>
-      <c r="N17" s="7">
+      <c r="N17" s="8">
         <v>97.0</v>
       </c>
-      <c r="O17" s="7">
+      <c r="O17" s="8">
         <v>74.05</v>
       </c>
-      <c r="P17" s="7">
+      <c r="P17" s="8">
         <v>36.74</v>
       </c>
-      <c r="Q17" s="7">
+      <c r="Q17" s="8">
         <v>36.74</v>
       </c>
-      <c r="R17" s="7">
+      <c r="R17" s="8">
         <v>0.97</v>
       </c>
-      <c r="S17" s="8">
+      <c r="S17" s="9">
         <v>1.0</v>
       </c>
-      <c r="T17" s="7">
+      <c r="T17" s="8">
         <v>1.03</v>
       </c>
-      <c r="U17" s="7">
+      <c r="U17" s="8">
         <v>0.76</v>
       </c>
-      <c r="V17" s="7">
+      <c r="V17" s="8">
         <v>0.38</v>
       </c>
-      <c r="W17" s="7">
+      <c r="W17" s="8">
         <v>0.01</v>
       </c>
-      <c r="X17" s="8">
+      <c r="X17" s="9">
         <v>11.0</v>
       </c>
-      <c r="Y17" s="7">
+      <c r="Y17" s="8">
         <v>11.34</v>
       </c>
-      <c r="Z17" s="7">
+      <c r="Z17" s="8">
         <v>8.4</v>
       </c>
-      <c r="AA17" s="7">
+      <c r="AA17" s="8">
         <v>4.17</v>
       </c>
-      <c r="AB17" s="7">
+      <c r="AB17" s="8">
         <v>0.11</v>
       </c>
-      <c r="AC17" s="9" t="s">
+      <c r="AC17" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="AD17" s="9" t="s">
+      <c r="AD17" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="AE17" s="13">
+      <c r="AE17" s="14">
         <v>7.0</v>
       </c>
-      <c r="AF17" s="10"/>
+      <c r="AF17" s="11"/>
     </row>
     <row r="18">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="8" t="s">
         <v>52</v>
       </c>
       <c r="B18" s="1" t="str">
         <f t="shared" si="1"/>
         <v>WGS2A8</v>
       </c>
-      <c r="C18" s="7" t="str">
+      <c r="C18" s="2" t="str">
         <f t="shared" si="2"/>
         <v>haploid</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="8">
         <v>384.0</v>
       </c>
-      <c r="E18" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="F18" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="G18" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="H18" s="7">
+      <c r="E18" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="F18" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="G18" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="H18" s="8">
         <v>3.84</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I18" s="8">
         <v>232.0</v>
       </c>
-      <c r="J18" s="7">
+      <c r="J18" s="8">
         <v>60.42</v>
       </c>
-      <c r="K18" s="7">
+      <c r="K18" s="8">
         <v>60.42</v>
       </c>
-      <c r="L18" s="7">
+      <c r="L18" s="8">
         <v>60.42</v>
       </c>
-      <c r="M18" s="7">
+      <c r="M18" s="8">
         <v>2.32</v>
       </c>
-      <c r="N18" s="7">
+      <c r="N18" s="8">
         <v>213.0</v>
       </c>
-      <c r="O18" s="7">
+      <c r="O18" s="8">
         <v>91.81</v>
       </c>
-      <c r="P18" s="7">
+      <c r="P18" s="8">
         <v>55.47</v>
       </c>
-      <c r="Q18" s="7">
+      <c r="Q18" s="8">
         <v>55.47</v>
       </c>
-      <c r="R18" s="7">
+      <c r="R18" s="8">
         <v>2.13</v>
       </c>
-      <c r="S18" s="8">
+      <c r="S18" s="9">
         <v>101.0</v>
       </c>
-      <c r="T18" s="7">
+      <c r="T18" s="8">
         <v>47.42</v>
       </c>
-      <c r="U18" s="7">
+      <c r="U18" s="8">
         <v>43.53</v>
       </c>
-      <c r="V18" s="7">
+      <c r="V18" s="8">
         <v>26.3</v>
       </c>
-      <c r="W18" s="7">
+      <c r="W18" s="8">
         <v>1.01</v>
       </c>
-      <c r="X18" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="Y18" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="Z18" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="AA18" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="AB18" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="AC18" s="9" t="s">
+      <c r="X18" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="Y18" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="Z18" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="AA18" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="AB18" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="AC18" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="AD18" s="9" t="s">
+      <c r="AD18" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="AE18" s="13">
+      <c r="AE18" s="14">
         <v>8.0</v>
       </c>
-      <c r="AF18" s="10"/>
+      <c r="AF18" s="11"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
@@ -2298,7 +2302,7 @@
         <f t="shared" si="1"/>
         <v>WGS2E9</v>
       </c>
-      <c r="C19" s="1" t="str">
+      <c r="C19" s="2" t="str">
         <f t="shared" si="2"/>
         <v>diploid</v>
       </c>
@@ -2347,7 +2351,7 @@
       <c r="R19" s="1">
         <v>26.63</v>
       </c>
-      <c r="S19" s="2">
+      <c r="S19" s="3">
         <v>0.0</v>
       </c>
       <c r="T19" s="1">
@@ -2362,7 +2366,7 @@
       <c r="W19" s="1">
         <v>0.0</v>
       </c>
-      <c r="X19" s="2">
+      <c r="X19" s="3">
         <v>524.0</v>
       </c>
       <c r="Y19" s="1">
@@ -2377,114 +2381,114 @@
       <c r="AB19" s="1">
         <v>5.24</v>
       </c>
-      <c r="AC19" s="3" t="s">
+      <c r="AC19" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AD19" s="3" t="s">
+      <c r="AD19" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AE19" s="12">
+      <c r="AE19" s="13">
         <v>9.0</v>
       </c>
-      <c r="AF19" s="5"/>
+      <c r="AF19" s="6"/>
     </row>
     <row r="20">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="8" t="s">
         <v>54</v>
       </c>
       <c r="B20" s="1" t="str">
         <f t="shared" si="1"/>
         <v>WGS2F9</v>
       </c>
-      <c r="C20" s="7" t="str">
+      <c r="C20" s="2" t="str">
         <f t="shared" si="2"/>
         <v>haploid</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="8">
         <v>928.0</v>
       </c>
-      <c r="E20" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="F20" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="G20" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="H20" s="7">
+      <c r="E20" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="F20" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="G20" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="H20" s="8">
         <v>9.27</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I20" s="8">
         <v>596.0</v>
       </c>
-      <c r="J20" s="7">
+      <c r="J20" s="8">
         <v>64.22</v>
       </c>
-      <c r="K20" s="7">
+      <c r="K20" s="8">
         <v>64.22</v>
       </c>
-      <c r="L20" s="7">
+      <c r="L20" s="8">
         <v>64.22</v>
       </c>
-      <c r="M20" s="7">
+      <c r="M20" s="8">
         <v>5.95</v>
       </c>
-      <c r="N20" s="7">
+      <c r="N20" s="8">
         <v>511.0</v>
       </c>
-      <c r="O20" s="7">
+      <c r="O20" s="8">
         <v>85.74</v>
       </c>
-      <c r="P20" s="7">
+      <c r="P20" s="8">
         <v>55.06</v>
       </c>
-      <c r="Q20" s="7">
+      <c r="Q20" s="8">
         <v>55.06</v>
       </c>
-      <c r="R20" s="7">
+      <c r="R20" s="8">
         <v>5.1</v>
       </c>
-      <c r="S20" s="8">
+      <c r="S20" s="9">
         <v>284.0</v>
       </c>
-      <c r="T20" s="7">
+      <c r="T20" s="8">
         <v>55.58</v>
       </c>
-      <c r="U20" s="7">
+      <c r="U20" s="8">
         <v>47.65</v>
       </c>
-      <c r="V20" s="7">
+      <c r="V20" s="8">
         <v>30.6</v>
       </c>
-      <c r="W20" s="7">
+      <c r="W20" s="8">
         <v>2.84</v>
       </c>
-      <c r="X20" s="8">
+      <c r="X20" s="9">
         <v>2.0</v>
       </c>
-      <c r="Y20" s="7">
+      <c r="Y20" s="8">
         <v>0.39</v>
       </c>
-      <c r="Z20" s="7">
+      <c r="Z20" s="8">
         <v>0.34</v>
       </c>
-      <c r="AA20" s="7">
+      <c r="AA20" s="8">
         <v>0.22</v>
       </c>
-      <c r="AB20" s="7">
+      <c r="AB20" s="8">
         <v>0.02</v>
       </c>
-      <c r="AC20" s="9" t="s">
+      <c r="AC20" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="AD20" s="9" t="s">
+      <c r="AD20" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="AE20" s="13">
+      <c r="AE20" s="14">
         <v>9.0</v>
       </c>
-      <c r="AF20" s="10"/>
+      <c r="AF20" s="11"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
@@ -2494,7 +2498,7 @@
         <f t="shared" si="1"/>
         <v>WGS2C11</v>
       </c>
-      <c r="C21" s="1" t="str">
+      <c r="C21" s="2" t="str">
         <f t="shared" si="2"/>
         <v>diploid</v>
       </c>
@@ -2543,7 +2547,7 @@
       <c r="R21" s="1">
         <v>1.53</v>
       </c>
-      <c r="S21" s="2">
+      <c r="S21" s="3">
         <v>0.0</v>
       </c>
       <c r="T21" s="1">
@@ -2558,7 +2562,7 @@
       <c r="W21" s="1">
         <v>0.0</v>
       </c>
-      <c r="X21" s="2">
+      <c r="X21" s="3">
         <v>32.0</v>
       </c>
       <c r="Y21" s="1">
@@ -2573,510 +2577,511 @@
       <c r="AB21" s="1">
         <v>0.32</v>
       </c>
-      <c r="AC21" s="3" t="s">
+      <c r="AC21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AD21" s="3" t="s">
+      <c r="AD21" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AE21" s="12">
+      <c r="AE21" s="13">
         <v>11.0</v>
       </c>
-      <c r="AF21" s="5"/>
+      <c r="AF21" s="6"/>
     </row>
     <row r="22">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="8" t="s">
         <v>56</v>
       </c>
       <c r="B22" s="1" t="str">
         <f t="shared" si="1"/>
         <v>WGS2E11</v>
       </c>
-      <c r="C22" s="7" t="str">
+      <c r="C22" s="2" t="str">
         <f t="shared" si="2"/>
         <v>haploid</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="8">
         <v>80.0</v>
       </c>
-      <c r="E22" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="F22" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="G22" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="H22" s="7">
+      <c r="E22" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="F22" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="G22" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="H22" s="8">
         <v>1.92</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="8">
         <v>39.0</v>
       </c>
-      <c r="J22" s="7">
+      <c r="J22" s="8">
         <v>48.75</v>
       </c>
-      <c r="K22" s="7">
+      <c r="K22" s="8">
         <v>48.75</v>
       </c>
-      <c r="L22" s="7">
+      <c r="L22" s="8">
         <v>48.75</v>
       </c>
-      <c r="M22" s="7">
+      <c r="M22" s="8">
         <v>0.93</v>
       </c>
-      <c r="N22" s="7">
+      <c r="N22" s="8">
         <v>36.0</v>
       </c>
-      <c r="O22" s="7">
+      <c r="O22" s="8">
         <v>92.31</v>
       </c>
-      <c r="P22" s="7">
+      <c r="P22" s="8">
         <v>45.0</v>
       </c>
-      <c r="Q22" s="7">
+      <c r="Q22" s="8">
         <v>45.0</v>
       </c>
-      <c r="R22" s="7">
+      <c r="R22" s="8">
         <v>0.86</v>
       </c>
-      <c r="S22" s="8">
+      <c r="S22" s="9">
         <v>6.0</v>
       </c>
-      <c r="T22" s="7">
+      <c r="T22" s="8">
         <v>16.67</v>
       </c>
-      <c r="U22" s="7">
+      <c r="U22" s="8">
         <v>15.38</v>
       </c>
-      <c r="V22" s="7">
+      <c r="V22" s="8">
         <v>7.5</v>
       </c>
-      <c r="W22" s="7">
+      <c r="W22" s="8">
         <v>0.14</v>
       </c>
-      <c r="X22" s="8">
+      <c r="X22" s="9">
         <v>2.0</v>
       </c>
-      <c r="Y22" s="7">
+      <c r="Y22" s="8">
         <v>5.56</v>
       </c>
-      <c r="Z22" s="7">
+      <c r="Z22" s="8">
         <v>5.13</v>
       </c>
-      <c r="AA22" s="7">
+      <c r="AA22" s="8">
         <v>2.5</v>
       </c>
-      <c r="AB22" s="7">
+      <c r="AB22" s="8">
         <v>0.05</v>
       </c>
-      <c r="AC22" s="9" t="s">
+      <c r="AC22" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="AD22" s="9" t="s">
+      <c r="AD22" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="AE22" s="13">
+      <c r="AE22" s="14">
         <v>11.0</v>
       </c>
-      <c r="AF22" s="10"/>
+      <c r="AF22" s="11"/>
     </row>
     <row r="23">
-      <c r="AC23" s="4"/>
-      <c r="AD23" s="4"/>
-      <c r="AE23" s="5"/>
-      <c r="AF23" s="5"/>
+      <c r="C23" s="2"/>
+      <c r="AC23" s="5"/>
+      <c r="AD23" s="5"/>
+      <c r="AE23" s="6"/>
+      <c r="AF23" s="6"/>
     </row>
     <row r="24">
-      <c r="AC24" s="4"/>
-      <c r="AD24" s="4"/>
-      <c r="AE24" s="5"/>
-      <c r="AF24" s="5"/>
+      <c r="AC24" s="5"/>
+      <c r="AD24" s="5"/>
+      <c r="AE24" s="6"/>
+      <c r="AF24" s="6"/>
     </row>
     <row r="25">
-      <c r="AC25" s="4"/>
-      <c r="AD25" s="4"/>
-      <c r="AE25" s="5"/>
-      <c r="AF25" s="5"/>
+      <c r="AC25" s="5"/>
+      <c r="AD25" s="5"/>
+      <c r="AE25" s="6"/>
+      <c r="AF25" s="6"/>
     </row>
     <row r="26">
-      <c r="AC26" s="4"/>
-      <c r="AD26" s="4"/>
-      <c r="AE26" s="14"/>
-      <c r="AF26" s="14"/>
+      <c r="AC26" s="5"/>
+      <c r="AD26" s="5"/>
+      <c r="AE26" s="15"/>
+      <c r="AF26" s="15"/>
     </row>
     <row r="27">
-      <c r="AC27" s="4"/>
-      <c r="AD27" s="4"/>
-      <c r="AE27" s="5"/>
-      <c r="AF27" s="5"/>
+      <c r="AC27" s="5"/>
+      <c r="AD27" s="5"/>
+      <c r="AE27" s="6"/>
+      <c r="AF27" s="6"/>
     </row>
     <row r="28">
-      <c r="AC28" s="4"/>
-      <c r="AD28" s="4"/>
-      <c r="AE28" s="5"/>
-      <c r="AF28" s="5"/>
+      <c r="AC28" s="5"/>
+      <c r="AD28" s="5"/>
+      <c r="AE28" s="6"/>
+      <c r="AF28" s="6"/>
     </row>
     <row r="29">
-      <c r="AC29" s="4"/>
-      <c r="AD29" s="4"/>
-      <c r="AE29" s="5"/>
-      <c r="AF29" s="5"/>
+      <c r="AC29" s="5"/>
+      <c r="AD29" s="5"/>
+      <c r="AE29" s="6"/>
+      <c r="AF29" s="6"/>
     </row>
     <row r="30">
-      <c r="AC30" s="4"/>
-      <c r="AD30" s="4"/>
-      <c r="AE30" s="5"/>
-      <c r="AF30" s="5"/>
+      <c r="AC30" s="5"/>
+      <c r="AD30" s="5"/>
+      <c r="AE30" s="6"/>
+      <c r="AF30" s="6"/>
     </row>
     <row r="31">
-      <c r="AC31" s="4"/>
-      <c r="AD31" s="4"/>
-      <c r="AE31" s="5"/>
-      <c r="AF31" s="5"/>
+      <c r="AC31" s="5"/>
+      <c r="AD31" s="5"/>
+      <c r="AE31" s="6"/>
+      <c r="AF31" s="6"/>
     </row>
     <row r="32">
-      <c r="AC32" s="4"/>
-      <c r="AD32" s="4"/>
-      <c r="AE32" s="5"/>
-      <c r="AF32" s="5"/>
+      <c r="AC32" s="5"/>
+      <c r="AD32" s="5"/>
+      <c r="AE32" s="6"/>
+      <c r="AF32" s="6"/>
     </row>
     <row r="33">
-      <c r="A33" s="15"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="16">
+      <c r="A33" s="16"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="17">
         <v>1.0</v>
       </c>
-      <c r="D33" s="16">
+      <c r="D33" s="17">
         <v>2.0</v>
       </c>
-      <c r="E33" s="16">
+      <c r="E33" s="17">
         <v>3.0</v>
       </c>
-      <c r="F33" s="16">
+      <c r="F33" s="17">
         <v>4.0</v>
       </c>
-      <c r="G33" s="16">
+      <c r="G33" s="17">
         <v>5.0</v>
       </c>
-      <c r="H33" s="16">
+      <c r="H33" s="17">
         <v>6.0</v>
       </c>
-      <c r="I33" s="16">
+      <c r="I33" s="17">
         <v>7.0</v>
       </c>
-      <c r="J33" s="16">
+      <c r="J33" s="17">
         <v>8.0</v>
       </c>
-      <c r="K33" s="16">
+      <c r="K33" s="17">
         <v>9.0</v>
       </c>
-      <c r="L33" s="16">
+      <c r="L33" s="17">
         <v>10.0</v>
       </c>
-      <c r="M33" s="16">
+      <c r="M33" s="17">
         <v>11.0</v>
       </c>
-      <c r="N33" s="16">
+      <c r="N33" s="17">
         <v>12.0</v>
       </c>
-      <c r="AC33" s="4"/>
-      <c r="AD33" s="4"/>
-      <c r="AE33" s="5"/>
-      <c r="AF33" s="5"/>
+      <c r="AC33" s="5"/>
+      <c r="AD33" s="5"/>
+      <c r="AE33" s="6"/>
+      <c r="AF33" s="6"/>
     </row>
     <row r="34">
-      <c r="A34" s="16" t="s">
+      <c r="A34" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="16"/>
-      <c r="C34" s="17">
+      <c r="B34" s="17"/>
+      <c r="C34" s="18">
         <v>1.0</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D34" s="18">
         <v>8.0</v>
       </c>
-      <c r="E34" s="17">
+      <c r="E34" s="18">
         <v>15.0</v>
       </c>
-      <c r="F34" s="17">
+      <c r="F34" s="18">
         <v>22.0</v>
       </c>
-      <c r="G34" s="17">
+      <c r="G34" s="18">
         <v>29.0</v>
       </c>
-      <c r="H34" s="17">
+      <c r="H34" s="18">
         <v>36.0</v>
       </c>
-      <c r="I34" s="17">
+      <c r="I34" s="18">
         <v>43.0</v>
       </c>
-      <c r="J34" s="17">
+      <c r="J34" s="18">
         <v>50.0</v>
       </c>
-      <c r="K34" s="17">
+      <c r="K34" s="18">
         <v>57.0</v>
       </c>
-      <c r="L34" s="17">
+      <c r="L34" s="18">
         <v>64.0</v>
       </c>
-      <c r="M34" s="17">
+      <c r="M34" s="18">
         <v>71.0</v>
       </c>
-      <c r="N34" s="17">
+      <c r="N34" s="18">
         <v>78.0</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="16"/>
-      <c r="C35" s="17">
+      <c r="B35" s="17"/>
+      <c r="C35" s="18">
         <v>2.0</v>
       </c>
-      <c r="D35" s="17">
+      <c r="D35" s="18">
         <v>9.0</v>
       </c>
-      <c r="E35" s="17">
+      <c r="E35" s="18">
         <v>16.0</v>
       </c>
-      <c r="F35" s="17">
+      <c r="F35" s="18">
         <v>23.0</v>
       </c>
-      <c r="G35" s="17">
+      <c r="G35" s="18">
         <v>30.0</v>
       </c>
-      <c r="H35" s="17">
+      <c r="H35" s="18">
         <v>37.0</v>
       </c>
-      <c r="I35" s="17">
+      <c r="I35" s="18">
         <v>44.0</v>
       </c>
-      <c r="J35" s="17">
+      <c r="J35" s="18">
         <v>51.0</v>
       </c>
-      <c r="K35" s="17">
+      <c r="K35" s="18">
         <v>58.0</v>
       </c>
-      <c r="L35" s="17">
+      <c r="L35" s="18">
         <v>65.0</v>
       </c>
-      <c r="M35" s="17">
+      <c r="M35" s="18">
         <v>72.0</v>
       </c>
-      <c r="N35" s="17">
+      <c r="N35" s="18">
         <v>79.0</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="16"/>
-      <c r="C36" s="17">
+      <c r="B36" s="17"/>
+      <c r="C36" s="18">
         <v>3.0</v>
       </c>
-      <c r="D36" s="17">
+      <c r="D36" s="18">
         <v>10.0</v>
       </c>
-      <c r="E36" s="17">
+      <c r="E36" s="18">
         <v>17.0</v>
       </c>
-      <c r="F36" s="17">
+      <c r="F36" s="18">
         <v>24.0</v>
       </c>
-      <c r="G36" s="17">
+      <c r="G36" s="18">
         <v>31.0</v>
       </c>
-      <c r="H36" s="17">
+      <c r="H36" s="18">
         <v>38.0</v>
       </c>
-      <c r="I36" s="17">
+      <c r="I36" s="18">
         <v>45.0</v>
       </c>
-      <c r="J36" s="17">
+      <c r="J36" s="18">
         <v>52.0</v>
       </c>
-      <c r="K36" s="17">
+      <c r="K36" s="18">
         <v>59.0</v>
       </c>
-      <c r="L36" s="17">
+      <c r="L36" s="18">
         <v>66.0</v>
       </c>
-      <c r="M36" s="17">
+      <c r="M36" s="18">
         <v>73.0</v>
       </c>
-      <c r="N36" s="17">
+      <c r="N36" s="18">
         <v>80.0</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="16" t="s">
+      <c r="A37" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="16"/>
-      <c r="C37" s="17">
+      <c r="B37" s="17"/>
+      <c r="C37" s="18">
         <v>4.0</v>
       </c>
-      <c r="D37" s="17">
+      <c r="D37" s="18">
         <v>11.0</v>
       </c>
-      <c r="E37" s="17">
+      <c r="E37" s="18">
         <v>18.0</v>
       </c>
-      <c r="F37" s="17">
+      <c r="F37" s="18">
         <v>25.0</v>
       </c>
-      <c r="G37" s="17">
+      <c r="G37" s="18">
         <v>32.0</v>
       </c>
-      <c r="H37" s="17">
+      <c r="H37" s="18">
         <v>39.0</v>
       </c>
-      <c r="I37" s="17">
+      <c r="I37" s="18">
         <v>46.0</v>
       </c>
-      <c r="J37" s="17">
+      <c r="J37" s="18">
         <v>53.0</v>
       </c>
-      <c r="K37" s="17">
+      <c r="K37" s="18">
         <v>60.0</v>
       </c>
-      <c r="L37" s="17">
+      <c r="L37" s="18">
         <v>67.0</v>
       </c>
-      <c r="M37" s="17">
+      <c r="M37" s="18">
         <v>74.0</v>
       </c>
-      <c r="N37" s="17">
+      <c r="N37" s="18">
         <v>81.0</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="16" t="s">
+      <c r="A38" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="16"/>
-      <c r="C38" s="17">
+      <c r="B38" s="17"/>
+      <c r="C38" s="18">
         <v>5.0</v>
       </c>
-      <c r="D38" s="17">
+      <c r="D38" s="18">
         <v>12.0</v>
       </c>
-      <c r="E38" s="17">
+      <c r="E38" s="18">
         <v>19.0</v>
       </c>
-      <c r="F38" s="17">
+      <c r="F38" s="18">
         <v>26.0</v>
       </c>
-      <c r="G38" s="17">
+      <c r="G38" s="18">
         <v>33.0</v>
       </c>
-      <c r="H38" s="17">
+      <c r="H38" s="18">
         <v>40.0</v>
       </c>
-      <c r="I38" s="17">
+      <c r="I38" s="18">
         <v>47.0</v>
       </c>
-      <c r="J38" s="17">
+      <c r="J38" s="18">
         <v>54.0</v>
       </c>
-      <c r="K38" s="17">
+      <c r="K38" s="18">
         <v>61.0</v>
       </c>
-      <c r="L38" s="17">
+      <c r="L38" s="18">
         <v>68.0</v>
       </c>
-      <c r="M38" s="17">
+      <c r="M38" s="18">
         <v>75.0</v>
       </c>
-      <c r="N38" s="17">
+      <c r="N38" s="18">
         <v>82.0</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="16" t="s">
+      <c r="A39" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="16"/>
-      <c r="C39" s="17">
+      <c r="B39" s="17"/>
+      <c r="C39" s="18">
         <v>6.0</v>
       </c>
-      <c r="D39" s="17">
+      <c r="D39" s="18">
         <v>13.0</v>
       </c>
-      <c r="E39" s="17">
+      <c r="E39" s="18">
         <v>20.0</v>
       </c>
-      <c r="F39" s="17">
+      <c r="F39" s="18">
         <v>27.0</v>
       </c>
-      <c r="G39" s="17">
+      <c r="G39" s="18">
         <v>34.0</v>
       </c>
-      <c r="H39" s="17">
+      <c r="H39" s="18">
         <v>41.0</v>
       </c>
-      <c r="I39" s="17">
+      <c r="I39" s="18">
         <v>48.0</v>
       </c>
-      <c r="J39" s="17">
+      <c r="J39" s="18">
         <v>55.0</v>
       </c>
-      <c r="K39" s="17">
+      <c r="K39" s="18">
         <v>62.0</v>
       </c>
-      <c r="L39" s="17">
+      <c r="L39" s="18">
         <v>69.0</v>
       </c>
-      <c r="M39" s="17">
+      <c r="M39" s="18">
         <v>76.0</v>
       </c>
-      <c r="N39" s="17">
+      <c r="N39" s="18">
         <v>83.0</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="16" t="s">
+      <c r="A40" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="16"/>
-      <c r="C40" s="17">
+      <c r="B40" s="17"/>
+      <c r="C40" s="18">
         <v>7.0</v>
       </c>
-      <c r="D40" s="17">
+      <c r="D40" s="18">
         <v>14.0</v>
       </c>
-      <c r="E40" s="17">
+      <c r="E40" s="18">
         <v>21.0</v>
       </c>
-      <c r="F40" s="17">
+      <c r="F40" s="18">
         <v>28.0</v>
       </c>
-      <c r="G40" s="17">
+      <c r="G40" s="18">
         <v>35.0</v>
       </c>
-      <c r="H40" s="17">
+      <c r="H40" s="18">
         <v>42.0</v>
       </c>
-      <c r="I40" s="17">
+      <c r="I40" s="18">
         <v>49.0</v>
       </c>
-      <c r="J40" s="17">
+      <c r="J40" s="18">
         <v>56.0</v>
       </c>
-      <c r="K40" s="17">
+      <c r="K40" s="18">
         <v>63.0</v>
       </c>
-      <c r="L40" s="17">
+      <c r="L40" s="18">
         <v>70.0</v>
       </c>
-      <c r="M40" s="17">
+      <c r="M40" s="18">
         <v>77.0</v>
       </c>
-      <c r="N40" s="17">
+      <c r="N40" s="18">
         <v>84.0</v>
       </c>
     </row>

</xml_diff>